<commit_message>
dev-1.0.0 : Update Templete dan Index Sales
</commit_message>
<xml_diff>
--- a/public/files/Template_Direct Material_New_2024_New.xlsx
+++ b/public/files/Template_Direct Material_New_2024_New.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Project Management\19_Cubic Pro\Templete yang akan digunakan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA913AA-AC25-4A97-A3B3-96FEA130A6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A34F7A7-3735-49BC-8AE9-74253A7747EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,10 +693,10 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q12" sqref="Q12"/>
+      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -793,9 +793,18 @@
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="4"/>
+      <c r="Q2" s="5">
+        <f t="shared" ref="Q2:Q28" si="0">SUM(E2:J2)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="5">
+        <f>SUM(K2:P2)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="4">
+        <f>Q2+R2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
@@ -822,9 +831,18 @@
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="4"/>
+      <c r="Q3" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="5">
+        <f t="shared" ref="R3:R10" si="1">SUM(K3:P3)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="4">
+        <f t="shared" ref="S3:S10" si="2">Q3+R3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
@@ -851,9 +869,18 @@
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="4"/>
+      <c r="Q4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
@@ -880,9 +907,18 @@
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="4"/>
+      <c r="Q5" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
@@ -909,9 +945,18 @@
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="4"/>
+      <c r="Q6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
@@ -938,9 +983,18 @@
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="4"/>
+      <c r="Q7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
@@ -967,9 +1021,18 @@
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="4"/>
+      <c r="Q8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
@@ -996,9 +1059,18 @@
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="4"/>
+      <c r="Q9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S9" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
@@ -1025,9 +1097,18 @@
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="4"/>
+      <c r="Q10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S10" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
@@ -1054,9 +1135,18 @@
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="4"/>
+      <c r="Q11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="5">
+        <f>SUM(K11:P11)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="4">
+        <f>Q11+R11</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
@@ -1083,9 +1173,18 @@
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="4"/>
+      <c r="Q12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="5">
+        <f t="shared" ref="R12:R19" si="3">SUM(K12:P12)</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" ref="S12:S19" si="4">Q12+R12</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
@@ -1112,9 +1211,18 @@
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="4"/>
+      <c r="Q13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
@@ -1141,9 +1249,18 @@
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="4"/>
+      <c r="Q14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
@@ -1170,9 +1287,18 @@
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="4"/>
+      <c r="Q15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
@@ -1199,9 +1325,18 @@
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="4"/>
+      <c r="Q16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
@@ -1228,9 +1363,18 @@
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="4"/>
+      <c r="Q17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
@@ -1257,9 +1401,18 @@
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="4"/>
+      <c r="Q18" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
@@ -1286,9 +1439,18 @@
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="4"/>
+      <c r="Q19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S19" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
@@ -1315,9 +1477,18 @@
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="4"/>
+      <c r="Q20" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="5">
+        <f>SUM(K20:P20)</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="4">
+        <f>Q20+R20</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
@@ -1344,9 +1515,18 @@
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="4"/>
+      <c r="Q21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="5">
+        <f t="shared" ref="R21:R28" si="5">SUM(K21:P21)</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="4">
+        <f t="shared" ref="S21:S28" si="6">Q21+R21</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
@@ -1373,9 +1553,18 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="4"/>
+      <c r="Q22" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S22" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
@@ -1402,9 +1591,18 @@
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
       <c r="P23" s="13"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="4"/>
+      <c r="Q23" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
@@ -1431,9 +1629,18 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="4"/>
+      <c r="Q24" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S24" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
@@ -1460,9 +1667,18 @@
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
       <c r="P25" s="13"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="4"/>
+      <c r="Q25" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S25" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
@@ -1489,9 +1705,18 @@
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="4"/>
+      <c r="Q26" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S26" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
@@ -1518,9 +1743,18 @@
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="4"/>
+      <c r="Q27" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="14">
@@ -1547,9 +1781,18 @@
       <c r="N28" s="16"/>
       <c r="O28" s="16"/>
       <c r="P28" s="16"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="2"/>
+      <c r="Q28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
dev 1.0.0: Adding filter by dept and update templete
</commit_message>
<xml_diff>
--- a/public/files/Template_Direct Material_New_2024_New.xlsx
+++ b/public/files/Template_Direct Material_New_2024_New.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Project Management\19_Cubic Pro\Templete yang akan digunakan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Project Management\19_Cubic Pro\New Templte 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A34F7A7-3735-49BC-8AE9-74253A7747EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68253A7C-6169-4525-AF0F-804B679BBB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">DM!$A$1:$F$325</definedName>
-    <definedName name="TblDM">'Direct Material'!$A$1:$P$28</definedName>
+    <definedName name="TblDM">'Direct Material'!$B$1:$Q$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="59">
   <si>
     <t>ACC CODE</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>DEPT</t>
+  </si>
+  <si>
+    <t>PUR1</t>
   </si>
 </sst>
 </file>
@@ -690,99 +696,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="16" width="14.54296875" customWidth="1"/>
-    <col min="17" max="19" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="17" width="14.54296875" customWidth="1"/>
+    <col min="18" max="20" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7">
+      <c r="F1" s="7">
         <v>45383</v>
       </c>
-      <c r="F1" s="7">
+      <c r="G1" s="7">
         <v>45413</v>
       </c>
-      <c r="G1" s="7">
+      <c r="H1" s="7">
         <v>45444</v>
       </c>
-      <c r="H1" s="7">
+      <c r="I1" s="7">
         <v>45474</v>
       </c>
-      <c r="I1" s="7">
+      <c r="J1" s="7">
         <v>45505</v>
       </c>
-      <c r="J1" s="7">
+      <c r="K1" s="7">
         <v>45536</v>
       </c>
-      <c r="K1" s="7">
+      <c r="L1" s="7">
         <v>45566</v>
       </c>
-      <c r="L1" s="7">
+      <c r="M1" s="7">
         <v>45597</v>
       </c>
-      <c r="M1" s="7">
+      <c r="N1" s="7">
         <v>45627</v>
       </c>
-      <c r="N1" s="7">
+      <c r="O1" s="7">
         <v>45658</v>
       </c>
-      <c r="O1" s="7">
+      <c r="P1" s="7">
         <v>45689</v>
       </c>
-      <c r="P1" s="7">
+      <c r="Q1" s="7">
         <v>45717</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="10">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="10">
         <v>5111410101</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="F2" s="12">
+        <v>1</v>
+      </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
@@ -793,33 +806,36 @@
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
-      <c r="Q2" s="5">
-        <f t="shared" ref="Q2:Q28" si="0">SUM(E2:J2)</f>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="5">
+        <f t="shared" ref="R2:R28" si="0">SUM(F2:K2)</f>
+        <v>1</v>
+      </c>
+      <c r="S2" s="5">
+        <f>SUM(L2:Q2)</f>
         <v>0</v>
       </c>
-      <c r="R2" s="5">
-        <f>SUM(K2:P2)</f>
-        <v>0</v>
-      </c>
-      <c r="S2" s="4">
-        <f>Q2+R2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="10">
+      <c r="T2" s="4">
+        <f>R2+S2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="10">
         <v>5111310101</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -831,33 +847,36 @@
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
-      <c r="Q3" s="5">
+      <c r="Q3" s="13"/>
+      <c r="R3" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R3" s="5">
-        <f t="shared" ref="R3:R10" si="1">SUM(K3:P3)</f>
+      <c r="S3" s="5">
+        <f t="shared" ref="S3:S10" si="1">SUM(L3:Q3)</f>
         <v>0</v>
       </c>
-      <c r="S3" s="4">
-        <f t="shared" ref="S3:S10" si="2">Q3+R3</f>
+      <c r="T3" s="4">
+        <f t="shared" ref="T3:T10" si="2">R3+S3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="10">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="10">
         <v>5112210101</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -869,33 +888,36 @@
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
-      <c r="Q4" s="5">
+      <c r="Q4" s="12"/>
+      <c r="R4" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R4" s="5">
+      <c r="S4" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S4" s="4">
+      <c r="T4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="10">
         <v>5116040101</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -907,33 +929,36 @@
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
-      <c r="Q5" s="5">
+      <c r="Q5" s="13"/>
+      <c r="R5" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R5" s="5">
+      <c r="S5" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S5" s="4">
+      <c r="T5" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="10">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="10">
         <v>5117010101</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -945,33 +970,36 @@
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
-      <c r="Q6" s="5">
+      <c r="Q6" s="12"/>
+      <c r="R6" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R6" s="5">
+      <c r="S6" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S6" s="4">
+      <c r="T6" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -983,33 +1011,36 @@
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
-      <c r="Q7" s="5">
+      <c r="Q7" s="13"/>
+      <c r="R7" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R7" s="5">
+      <c r="S7" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S7" s="4">
+      <c r="T7" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -1021,33 +1052,36 @@
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
-      <c r="Q8" s="5">
+      <c r="Q8" s="12"/>
+      <c r="R8" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R8" s="5">
+      <c r="S8" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S8" s="4">
+      <c r="T8" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="10">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="10">
         <v>5112410101</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -1059,33 +1093,36 @@
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
-      <c r="Q9" s="5">
+      <c r="Q9" s="13"/>
+      <c r="R9" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R9" s="5">
+      <c r="S9" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S9" s="4">
+      <c r="T9" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="10">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="10">
         <v>4315060101</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -1097,33 +1134,36 @@
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
-      <c r="Q10" s="5">
+      <c r="Q10" s="12"/>
+      <c r="R10" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R10" s="5">
+      <c r="S10" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S10" s="4">
+      <c r="T10" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="10">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="10">
         <v>5111410101</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -1135,33 +1175,36 @@
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
-      <c r="Q11" s="5">
+      <c r="Q11" s="13"/>
+      <c r="R11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R11" s="5">
-        <f>SUM(K11:P11)</f>
+      <c r="S11" s="5">
+        <f>SUM(L11:Q11)</f>
         <v>0</v>
       </c>
-      <c r="S11" s="4">
-        <f>Q11+R11</f>
+      <c r="T11" s="4">
+        <f>R11+S11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="10">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="10">
         <v>5111310101</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -1173,33 +1216,36 @@
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
-      <c r="Q12" s="5">
+      <c r="Q12" s="12"/>
+      <c r="R12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R12" s="5">
-        <f t="shared" ref="R12:R19" si="3">SUM(K12:P12)</f>
+      <c r="S12" s="5">
+        <f t="shared" ref="S12:S19" si="3">SUM(L12:Q12)</f>
         <v>0</v>
       </c>
-      <c r="S12" s="4">
-        <f t="shared" ref="S12:S19" si="4">Q12+R12</f>
+      <c r="T12" s="4">
+        <f t="shared" ref="T12:T19" si="4">R12+S12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="10">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="10">
         <v>5112210101</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -1211,33 +1257,36 @@
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
-      <c r="Q13" s="5">
+      <c r="Q13" s="13"/>
+      <c r="R13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R13" s="5">
+      <c r="S13" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S13" s="4">
+      <c r="T13" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="10">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="10">
         <v>5116040101</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -1249,33 +1298,36 @@
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
-      <c r="Q14" s="5">
+      <c r="Q14" s="12"/>
+      <c r="R14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R14" s="5">
+      <c r="S14" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S14" s="4">
+      <c r="T14" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="10">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="10">
         <v>5117010101</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -1287,33 +1339,36 @@
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
-      <c r="Q15" s="5">
+      <c r="Q15" s="13"/>
+      <c r="R15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R15" s="5">
+      <c r="S15" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S15" s="4">
+      <c r="T15" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="C16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -1325,33 +1380,36 @@
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
-      <c r="Q16" s="5">
+      <c r="Q16" s="12"/>
+      <c r="R16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R16" s="5">
+      <c r="S16" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S16" s="4">
+      <c r="T16" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
@@ -1363,33 +1421,36 @@
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
-      <c r="Q17" s="5">
+      <c r="Q17" s="13"/>
+      <c r="R17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R17" s="5">
+      <c r="S17" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S17" s="4">
+      <c r="T17" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="10">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="10">
         <v>5112410101</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
@@ -1401,33 +1462,36 @@
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
-      <c r="Q18" s="5">
+      <c r="Q18" s="12"/>
+      <c r="R18" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R18" s="5">
+      <c r="S18" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S18" s="4">
+      <c r="T18" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="10">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="10">
         <v>4315060101</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
@@ -1439,33 +1503,36 @@
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
-      <c r="Q19" s="5">
+      <c r="Q19" s="13"/>
+      <c r="R19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R19" s="5">
+      <c r="S19" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S19" s="4">
+      <c r="T19" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="10">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="10">
         <v>5111410101</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="D20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
@@ -1477,33 +1544,36 @@
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
-      <c r="Q20" s="5">
+      <c r="Q20" s="12"/>
+      <c r="R20" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R20" s="5">
-        <f>SUM(K20:P20)</f>
+      <c r="S20" s="5">
+        <f>SUM(L20:Q20)</f>
         <v>0</v>
       </c>
-      <c r="S20" s="4">
-        <f>Q20+R20</f>
+      <c r="T20" s="4">
+        <f>R20+S20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="10">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="10">
         <v>5111310101</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="D21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
@@ -1515,33 +1585,36 @@
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13"/>
-      <c r="Q21" s="5">
+      <c r="Q21" s="13"/>
+      <c r="R21" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R21" s="5">
-        <f t="shared" ref="R21:R28" si="5">SUM(K21:P21)</f>
+      <c r="S21" s="5">
+        <f t="shared" ref="S21:S28" si="5">SUM(L21:Q21)</f>
         <v>0</v>
       </c>
-      <c r="S21" s="4">
-        <f t="shared" ref="S21:S28" si="6">Q21+R21</f>
+      <c r="T21" s="4">
+        <f t="shared" ref="T21:T28" si="6">R21+S21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="10">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="10">
         <v>5112210101</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="D22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
@@ -1553,33 +1626,36 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
-      <c r="Q22" s="5">
+      <c r="Q22" s="12"/>
+      <c r="R22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R22" s="5">
+      <c r="S22" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S22" s="4">
+      <c r="T22" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="10">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="10">
         <v>5116040101</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="D23" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
@@ -1591,33 +1667,36 @@
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
       <c r="P23" s="13"/>
-      <c r="Q23" s="5">
+      <c r="Q23" s="13"/>
+      <c r="R23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R23" s="5">
+      <c r="S23" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S23" s="4">
+      <c r="T23" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="10">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="10">
         <v>5117010101</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="D24" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
@@ -1629,33 +1708,36 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
-      <c r="Q24" s="5">
+      <c r="Q24" s="12"/>
+      <c r="R24" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R24" s="5">
+      <c r="S24" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S24" s="4">
+      <c r="T24" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="D25" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
@@ -1667,33 +1749,36 @@
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
       <c r="P25" s="13"/>
-      <c r="Q25" s="5">
+      <c r="Q25" s="13"/>
+      <c r="R25" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R25" s="5">
+      <c r="S25" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S25" s="4">
+      <c r="T25" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="D26" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
@@ -1705,33 +1790,36 @@
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
-      <c r="Q26" s="5">
+      <c r="Q26" s="12"/>
+      <c r="R26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R26" s="5">
+      <c r="S26" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S26" s="4">
+      <c r="T26" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="10">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="10">
         <v>5112410101</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="C27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="D27" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
@@ -1743,33 +1831,36 @@
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13"/>
-      <c r="Q27" s="5">
+      <c r="Q27" s="13"/>
+      <c r="R27" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R27" s="5">
+      <c r="S27" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S27" s="4">
+      <c r="T27" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="14">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A28" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="14">
         <v>4315060101</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="C28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="D28" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
@@ -1781,15 +1872,16 @@
       <c r="N28" s="16"/>
       <c r="O28" s="16"/>
       <c r="P28" s="16"/>
-      <c r="Q28" s="3">
+      <c r="Q28" s="16"/>
+      <c r="R28" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R28" s="3">
+      <c r="S28" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S28" s="2">
+      <c r="T28" s="2">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -1798,7 +1890,7 @@
   <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <protectedRanges>
     <protectedRange sqref="A29:XFD139" name="OPEN 2"/>
-    <protectedRange sqref="E2:P1048576" name="OPEN 1"/>
+    <protectedRange sqref="F2:Q1048576" name="OPEN 1"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>